<commit_message>
code update for null result
</commit_message>
<xml_diff>
--- a/src/main/resources/sql/ChatRequirements.xlsx
+++ b/src/main/resources/sql/ChatRequirements.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8445"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="28125" windowHeight="5880" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Possible_Chat_Queries" sheetId="1" r:id="rId1"/>
     <sheet name="Tables" sheetId="2" r:id="rId2"/>
     <sheet name="Working_Queries" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L20"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1011,7 +1012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1019,14 +1020,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1299,7 +1301,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1309,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,16 +1340,16 @@
       <c r="D1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
       <c r="N1" s="1" t="s">
         <v>77</v>
       </c>
@@ -3106,8 +3108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,362 +3119,362 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="11">
         <v>13</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="11">
         <v>14</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="11">
         <v>15</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <v>16</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <v>17</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="8">
         <v>18</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="8">
         <v>19</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>20</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="8">
         <v>21</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="8">
         <v>22</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="A25" s="8">
         <v>23</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="A26" s="11">
         <v>24</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="8">
         <v>25</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="A28" s="8">
         <v>26</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="11">
         <v>27</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="A30" s="8">
         <v>28</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="A31" s="8">
         <v>29</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="A32" s="8">
         <v>30</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="9" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="A33" s="8">
         <v>31</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+      <c r="A34" s="8">
         <v>32</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="9" t="s">
         <v>247</v>
       </c>
     </row>

</xml_diff>